<commit_message>
Adjusted the second prompt and the validation tests.
</commit_message>
<xml_diff>
--- a/data/validation sample/validation results/original.xlsx
+++ b/data/validation sample/validation results/original.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -826,7 +826,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1658736242723</t>
+          <t>1658736030850</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -846,29 +846,29 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4e</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1658760534237</t>
+          <t>1658736242723</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -878,34 +878,34 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>12</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1658761359618</t>
+          <t>1658760534237</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -915,29 +915,29 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>1, 2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>4d</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1658332402648</t>
+          <t>1658761359618</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -952,7 +952,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1, 2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -974,12 +974,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1658932859587</t>
+          <t>1658332363822</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -994,24 +994,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>4d</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>1658918012431</t>
+          <t>1658332402648</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>4c</t>
+          <t>4d</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1048,17 +1048,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1659344123097</t>
+          <t>1658828890713</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>8b</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1085,12 +1085,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1659613268597</t>
+          <t>1658916484762</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1100,12 +1100,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1115,34 +1115,34 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1660135979838</t>
+          <t>1658918012431</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4c</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1152,24 +1152,24 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1660292547743</t>
+          <t>1658920688970</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1179,24 +1179,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>1660825903929</t>
+          <t>1659087654686</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1211,12 +1211,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3, 9</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1226,19 +1226,19 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1663072313013</t>
+          <t>1659344123097</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1248,34 +1248,39 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>4d</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>1663072962898</t>
+          <t>1659697068194</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1285,7 +1290,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>4c</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1295,14 +1300,14 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1664284436141</t>
+          <t>1660135979838</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1317,12 +1322,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1339,17 +1344,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1664284677736</t>
+          <t>1660292547743</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1359,29 +1364,29 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>1664356559124</t>
+          <t>1660825903929</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1396,7 +1401,12 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>4</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1408,17 +1418,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1664358119728</t>
+          <t>1661251238333</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1428,34 +1438,34 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>A</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1668780056167</t>
+          <t>1661853748366</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>8b</t>
+          <t>11</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1465,7 +1475,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4d</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1475,14 +1485,14 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1668781989003</t>
+          <t>1663072313013</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1497,7 +1507,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1514,27 +1524,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1669281355185</t>
+          <t>1663072962898</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3a</t>
+          <t>9</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1551,7 +1561,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1669284735935</t>
+          <t>1664284436141</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1571,7 +1581,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1588,12 +1598,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>1658736030850</t>
+          <t>1664284677736</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1603,12 +1613,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -1625,17 +1635,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1661251238333</t>
+          <t>1664285824607</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1645,54 +1655,557 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>5</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>13</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>1664356543473</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>1664356559124</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>1664356571739</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>1664356649635</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>1664358119728</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>1664358454304</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
           <t>1666263595546</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>4d</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>1</t>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>3a</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>1666255758576</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>1666266085050</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>3a</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>1666267003464</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>4e</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>1668780056167</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>8b</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>1668781989003</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>ND</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>1669281355185</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>3a</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>1669283492983</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>1669284735935</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>13</t>
         </is>
       </c>
     </row>

</xml_diff>